<commit_message>
carga web con flujo drive
</commit_message>
<xml_diff>
--- a/Clases.xlsx
+++ b/Clases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\ESCRITORIO HP\R_packages\CursoExperimentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\ESCRITORIO HP\R_packages\WCDECS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE1BEAC-CEE3-4136-B77A-A12A2430EEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2116038-D57A-42DB-9D5A-0A6F4D6518CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3292" yWindow="1853" windowWidth="18000" windowHeight="9397" xr2:uid="{38AD5D95-C7EC-4A58-AFC7-95892A1782E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{38AD5D95-C7EC-4A58-AFC7-95892A1782E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,20 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>Tema</t>
   </si>
   <si>
-    <t>Slide</t>
-  </si>
-  <si>
-    <t>Labs</t>
-  </si>
-  <si>
-    <t>add</t>
-  </si>
-  <si>
     <t>Inferencia causal</t>
   </si>
   <si>
@@ -77,7 +68,16 @@
     <t>Módulo</t>
   </si>
   <si>
-    <t>[ff](https://github.com/Nicolas-Schmidt/CursoExperimentos/blob/master/Programa/Programa2023.pdf)</t>
+    <t>[Slide 1](https://drive.google.com/file/d/11S5sW3UUnEfDna5LPVoeTchjwbAmg1iw/view?usp=sharing)</t>
+  </si>
+  <si>
+    <t>Presentaciones</t>
+  </si>
+  <si>
+    <t>Laboratorios</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -429,115 +429,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93399269-1F99-462F-8F16-46DE19A2F964}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="18.86328125" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
       <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
carga web con flujo drive2
</commit_message>
<xml_diff>
--- a/Clases.xlsx
+++ b/Clases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\ESCRITORIO HP\R_packages\WCDECS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2116038-D57A-42DB-9D5A-0A6F4D6518CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E0DD4E-C27F-4F25-AA14-FE59B8738CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{38AD5D95-C7EC-4A58-AFC7-95892A1782E5}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>Módulo</t>
   </si>
   <si>
-    <t>[Slide 1](https://drive.google.com/file/d/11S5sW3UUnEfDna5LPVoeTchjwbAmg1iw/view?usp=sharing)</t>
-  </si>
-  <si>
     <t>Presentaciones</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>[Slide 1](https://drive.google.com/file/d/1zpyLVzf75A1yy5zIeg0aAMfdiT24G651/view?usp=sharing)</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,10 +451,10 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -468,10 +468,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -485,10 +485,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -502,10 +502,10 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -519,10 +519,10 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -536,10 +536,10 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -553,10 +553,10 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -570,10 +570,10 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
typo slides inferencia causal
</commit_message>
<xml_diff>
--- a/Clases.xlsx
+++ b/Clases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/slopezcariboni/Google Drive/Experimentos dECON/Curso_Experimentos WEB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6F4CC6-55DF-9C43-94E3-591BDFF54273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12A2A98-C779-4E49-8FBC-4BCE4E8CCA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="31000" windowHeight="20120" xr2:uid="{38AD5D95-C7EC-4A58-AFC7-95892A1782E5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34780" windowHeight="25520" xr2:uid="{38AD5D95-C7EC-4A58-AFC7-95892A1782E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>Tema</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Pre-registro de experimentos</t>
   </si>
   <si>
-    <t>Cantidad de clases</t>
-  </si>
-  <si>
     <t>Módulo</t>
   </si>
   <si>
@@ -77,6 +74,9 @@
   </si>
   <si>
     <t>Lab 1: Introducción a la aleatorización simple,completa, y por bloques: [HTML](https://drive.google.com/u/0/uc?id=1A4J-XZab1r_iaJ9XU18nphHLtWFuFJSt&amp;export=download), [Rmd](https://drive.google.com/u/0/uc?id=19z4SL9vYMvSU8s1QrE_ICsWRCQWTeqvW&amp;export=download)</t>
+  </si>
+  <si>
+    <t>Lecturas</t>
   </si>
 </sst>
 </file>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93399269-1F99-462F-8F16-46DE19A2F964}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -442,19 +442,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -464,14 +464,14 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -481,14 +481,14 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
+      <c r="C3" t="s">
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -498,14 +498,14 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>2</v>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -515,14 +515,14 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
-        <v>4</v>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -532,14 +532,14 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>3</v>
+      <c r="C6" t="s">
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -549,14 +549,14 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
-        <v>3</v>
+      <c r="C7" t="s">
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -566,14 +566,14 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
-        <v>1</v>
+      <c r="C8" t="s">
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
carpeta en tema 1 de slides
</commit_message>
<xml_diff>
--- a/Clases.xlsx
+++ b/Clases.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/slopezcariboni/Google Drive/Experimentos dECON/Curso_Experimentos WEB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\1ry4DW0ytzBTm2QpZbBJtiQ_i_FWgsO8E\Experimentos dECON\Curso_Experimentos WEB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B812C6AD-3175-1749-B8E8-95D970BD7347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34780" windowHeight="25520" xr2:uid="{38AD5D95-C7EC-4A58-AFC7-95892A1782E5}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="34785" windowHeight="25515"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -79,13 +78,13 @@
     <t>Lab 1: Introducción a la aleatorización simple,completa, y por bloques: [HTML](https://drive.google.com/u/0/uc?id=1J6pjygV39O6g-A_VqCOC-A64s9vlZSd_&amp;export=download), [Rmd](https://drive.google.com/u/0/uc?id=1JAns64_qRpMvtEWVIQC39CLFNQhEMoCz&amp;export=download)</t>
   </si>
   <si>
-    <t>Gerber  &amp; Green 2012. FEDAI [Descarga](https://drive.google.com/drive/folders/14HDw0lx7v8cduNtj2XNvvZ5fm_lQ7Z6y?usp=sharing), Barbas 2010 [pdf](url)</t>
+    <t>Gerber  &amp; Green 2012. FEDAI [Descarga](https://drive.google.com/drive/folders/14HDw0lx7v8cduNtj2XNvvZ5fm_lQ7Z6y?usp=sharing), Barbas 2010 [pdf](https://drive.google.com/file/d/15SqCaheQIA_Eg8Q6CxkkF5Gdt2dPdK1Y/view)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -433,21 +432,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93399269-1F99-462F-8F16-46DE19A2F964}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="3" width="99.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="99.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -464,7 +463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -481,7 +480,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -498,7 +497,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -515,7 +514,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -532,7 +531,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -549,7 +548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -566,7 +565,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
lucia cambia xls de clases
</commit_message>
<xml_diff>
--- a/Clases.xlsx
+++ b/Clases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Docencia\2023\Curso Diseño de Experimentos\Curso_Experimentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/slopezcariboni/Google Drive/Experimentos dECON/Curso_Experimentos WEB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A913F3-BD33-432D-950F-B9E339EAA220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00185899-2CF2-B74D-A863-5D55FA6AA9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,8 +73,7 @@
   </si>
   <si>
     <t>Gerber  &amp; Green 2012. FEDAI [Descarga] https://drive.google.com/drive/folders/14HDw0lx7v8cduNtj2XNvvZ5fm_lQ7Z6y?usp=sharing)
-Barabas 2010 [pdf](https://drive.google.com/file/d/15SqCaheQIA_Eg8Q6CxkkF5Gdt2dPdK1Y/view)
-Aronow et al 2015 [pdf](url)</t>
+Barabas 2010 [pdf](https://drive.google.com/file/d/15SqCaheQIA_Eg8Q6CxkkF5Gdt2dPdK1Y/view), Aronow et al 2015 [pdf](url)</t>
   </si>
 </sst>
 </file>
@@ -432,18 +431,18 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7265625" customWidth="1"/>
-    <col min="3" max="3" width="85.81640625" customWidth="1"/>
-    <col min="4" max="4" width="80.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="85.83203125" customWidth="1"/>
+    <col min="4" max="4" width="80.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -460,7 +459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -477,7 +476,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -494,7 +493,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -511,7 +510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -528,7 +527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -545,7 +544,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -562,7 +561,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
tipos de experimentos correcto
</commit_message>
<xml_diff>
--- a/Clases.xlsx
+++ b/Clases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/slopezcariboni/Google Drive/Experimentos dECON/Curso_Experimentos WEB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\ESCRITORIO HP\R_packages\WCDECS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA0AB29-EC46-EA4C-85DD-72DB2CF6EBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CCD1BC-1B6E-426A-9D66-1BD652C2E3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32380" windowHeight="21200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
     <t>[Diseños de Aliento (IV).pdf](https://drive.google.com/uc?id=1GibnDUaXJoRjbGAnm3xDAFuwEVefa9WL&amp;export=download) [Diseños factoriales.pdf](https://drive.google.com/file/d/1AKmQLHQ-yn9fB0533-gTXhF1XAVFuGpG/view?usp=sharing) [Mediacion.pdf](https://drive.google.com/file/d/1BmkVIionkJ_jr30WgVESpIZJk3yt420d/view?usp=sharing); [VIDEO: clase diseños factoriales](https://salavirtual-udelar.zoom.us/rec/share/GGGdhrxRmmn4BtdejhVPfVMs6ZeGZC0Sa8T8VaHEhGnVUglTvuKT9rfqpRkV0ux5.AGyMPixdrmpWu4dv)</t>
   </si>
   <si>
-    <t>[Experimentos de Encuestas - Qualtrics](https://drive.google.com/file/d/10GOzGsxcG_Kb93XEzRaefCPD4RGQr1Ut/view?usp=sharing); [Tipos de Experimentos](https://drive.google.com/file/d/10A4EJFGWfebygOzYqxJxFSMew-zIN9r7/view?usp=sharing); [Experimentos de laboratorio](https://drive.google.com/file/d/1iVrSDTSJtu4G7u-j2Tg7Wm0kZPZryBSS/view?usp=sharing), [Experimentos Naturales con RDD.pdf](https://drive.google.com/file/d/1DDAqPEdh-ytKcQ9ri7y0a2KUzQ5ZrTpl/view?usp=sharing); [VIDEO: clase RDD y Experimentos de laboratorio](https://salavirtual-udelar.zoom.us/rec/share/hQFQRPxFhYmKtyHHAIt1WDRQHSY9Ve-MwOqTzys59zHZjm5voHeYg7gQSG3ztgzn.S4HDFr5gU2VSAAj0)</t>
+    <t>[Experimentos de Encuestas - Qualtrics](https://drive.google.com/file/d/10GOzGsxcG_Kb93XEzRaefCPD4RGQr1Ut/view?usp=sharing); [Tipos de Experimentos](https://drive.google.com/file/d/10NvXg9FUUU0muewzUiHE0CgGXWOo_wpK/view?usp=sharing); [Experimentos de laboratorio](https://drive.google.com/file/d/1iVrSDTSJtu4G7u-j2Tg7Wm0kZPZryBSS/view?usp=sharing), [Experimentos Naturales con RDD.pdf](https://drive.google.com/file/d/1DDAqPEdh-ytKcQ9ri7y0a2KUzQ5ZrTpl/view?usp=sharing); [VIDEO: clase RDD y Experimentos de laboratorio](https://salavirtual-udelar.zoom.us/rec/share/hQFQRPxFhYmKtyHHAIt1WDRQHSY9Ve-MwOqTzys59zHZjm5voHeYg7gQSG3ztgzn.S4HDFr5gU2VSAAj0)</t>
   </si>
 </sst>
 </file>
@@ -484,18 +484,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="36.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="36.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="36.33203125" style="1"/>
+    <col min="1" max="3" width="36.28515625" style="1"/>
     <col min="4" max="4" width="86" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="36.33203125" style="1"/>
+    <col min="5" max="16384" width="36.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -512,7 +512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -529,7 +529,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="69.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -546,7 +546,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="304" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="315" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -563,7 +563,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="240" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -580,7 +580,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -597,7 +597,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -614,7 +614,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>

</xml_diff>